<commit_message>
added third draft keywords
</commit_message>
<xml_diff>
--- a/assets/keywords.xlsx
+++ b/assets/keywords.xlsx
@@ -5,18 +5,19 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnandarL\source\repos\SHK-AIRI-Fundamentals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnandarL\Documents\semester5\SKH Forschungsprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13572"/>
   </bookViews>
   <sheets>
-    <sheet name="Second Draft" sheetId="6" r:id="rId1"/>
-    <sheet name="First Draft" sheetId="1" r:id="rId2"/>
-    <sheet name="SchmidtLampe" sheetId="2" r:id="rId3"/>
-    <sheet name="WolfVitale" sheetId="4" r:id="rId4"/>
-    <sheet name="Anandarajah" sheetId="5" r:id="rId5"/>
+    <sheet name="Third Draft" sheetId="7" r:id="rId1"/>
+    <sheet name="Second Draft" sheetId="6" r:id="rId2"/>
+    <sheet name="First Draft" sheetId="1" r:id="rId3"/>
+    <sheet name="SchmidtLampe" sheetId="2" r:id="rId4"/>
+    <sheet name="WolfVitale" sheetId="4" r:id="rId5"/>
+    <sheet name="Anandarajah" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="562">
   <si>
     <t>Digitalisierung</t>
   </si>
@@ -1674,9 +1675,6 @@
     <t>assistive technology</t>
   </si>
   <si>
-    <t>Algorithmus</t>
-  </si>
-  <si>
     <t>Rückführung</t>
   </si>
   <si>
@@ -1741,6 +1739,12 @@
   </si>
   <si>
     <t>classification methods</t>
+  </si>
+  <si>
+    <t>Internet of Things</t>
+  </si>
+  <si>
+    <t>Business-Process-AI</t>
   </si>
 </sst>
 </file>
@@ -1807,7 +1811,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1832,6 +1836,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1845,7 +1873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1860,11 +1888,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2205,20 +2240,1439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN191"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.09765625" customWidth="1"/>
+    <col min="2" max="2" width="19.09765625" customWidth="1"/>
+    <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>510</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>520</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>540</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>475</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>542</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>543</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>491</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>513</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>525</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>544</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>514</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>492</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>515</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>526</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>545</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>546</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>435</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>516</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>527</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>481</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>550</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>551</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>552</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>441</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>425</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>529</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>553</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="12" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>554</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="12" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>426</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>421</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="11" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="12" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>415</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="12" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="11"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="11" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="11"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>458</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="11"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="12" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="11" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="11"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>555</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="12" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="11"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="12" t="s">
+        <v>350</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="11"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="11" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="11"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>438</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="11" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="11"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="12" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="11"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="11"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E57" s="11"/>
+      <c r="F57" s="12" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="11"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>436</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="11"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="11"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="11"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="11"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="E60" s="3"/>
+      <c r="F60" s="11"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="11"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>396</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="11"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="11"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="E62" s="3"/>
+      <c r="F62" s="11"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="11"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="E63" s="3"/>
+      <c r="F63" s="11"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="11"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="E64" s="3"/>
+      <c r="F64" s="11"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="11"/>
+      <c r="B65" s="3"/>
+      <c r="D65" s="13" t="s">
+        <v>557</v>
+      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="11"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="11"/>
+      <c r="B66" s="3"/>
+      <c r="D66" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="11"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="11"/>
+      <c r="B67" s="3"/>
+      <c r="D67" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="11"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="11"/>
+      <c r="B68" s="3"/>
+      <c r="D68" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="11"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="11"/>
+      <c r="B69" s="3"/>
+      <c r="D69" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="11"/>
+      <c r="B70" s="3"/>
+      <c r="D70" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="D71" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="D72" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="11" t="s">
+        <v>417</v>
+      </c>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="12" t="s">
+        <v>334</v>
+      </c>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="13" t="s">
+        <v>558</v>
+      </c>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="11" t="s">
+        <v>419</v>
+      </c>
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="E87" s="3"/>
+      <c r="F87" s="3"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="D88" s="11" t="s">
+        <v>442</v>
+      </c>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D89" s="11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D90" s="11" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D91" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D92" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D93" s="11" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D94" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D95" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D96" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AN190"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.8984375" style="9" customWidth="1"/>
     <col min="2" max="3" width="27.59765625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="32.59765625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="25.69921875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32" style="9" customWidth="1"/>
+    <col min="5" max="5" width="25.3984375" style="9" customWidth="1"/>
     <col min="6" max="6" width="16.5" style="9" customWidth="1"/>
-    <col min="7" max="7" width="23.296875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="23.19921875" style="9" customWidth="1"/>
     <col min="8" max="16384" width="10.69921875" style="9"/>
   </cols>
   <sheetData>
@@ -2287,7 +3741,7 @@
         <v>358</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>288</v>
@@ -2331,26 +3785,26 @@
       <c r="AN2" s="3"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>538</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="12" t="s">
         <v>368</v>
       </c>
       <c r="G3" s="11"/>
-      <c r="H3" s="3"/>
+      <c r="H3" s="11"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -2391,22 +3845,21 @@
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="13" t="s">
         <v>517</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>91</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -2442,25 +3895,24 @@
       <c r="A5" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>357</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="13" t="s">
         <v>493</v>
       </c>
       <c r="G5" s="11"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
@@ -2493,19 +3945,19 @@
       <c r="AN5" s="3"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>472</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="13" t="s">
         <v>518</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>539</v>
-      </c>
-      <c r="E6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>510</v>
       </c>
       <c r="F6" s="11" t="s">
@@ -2550,14 +4002,14 @@
       <c r="A7" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="9" t="s">
         <v>519</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>88</v>
+      <c r="D7" s="13" t="s">
+        <v>539</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>71</v>
@@ -2601,22 +4053,22 @@
       <c r="AN7" s="3"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>474</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="12" t="s">
         <v>348</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="13" t="s">
         <v>494</v>
       </c>
       <c r="G8" s="11"/>
@@ -2664,8 +4116,8 @@
       <c r="C9" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>80</v>
+      <c r="D9" s="13" t="s">
+        <v>540</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>72</v>
@@ -2709,22 +4161,22 @@
       <c r="AN9" s="3"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="13" t="s">
         <v>489</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>512</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="13" t="s">
         <v>495</v>
       </c>
       <c r="G10" s="11"/>
@@ -2773,7 +4225,7 @@
         <v>522</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>103</v>
+        <v>403</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>76</v>
@@ -2820,19 +4272,19 @@
       <c r="A12" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>301</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>541</v>
+      <c r="D12" s="13" t="s">
+        <v>542</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="13" t="s">
         <v>496</v>
       </c>
       <c r="G12" s="11"/>
@@ -2871,7 +4323,7 @@
       <c r="AN12" s="3"/>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="13" t="s">
         <v>476</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -2880,8 +4332,8 @@
       <c r="C13" s="11" t="s">
         <v>521</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>542</v>
+      <c r="D13" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>186</v>
@@ -2928,14 +4380,14 @@
       <c r="A14" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="13" t="s">
         <v>490</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>403</v>
+      <c r="D14" s="13" t="s">
+        <v>543</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>170</v>
@@ -2979,7 +4431,7 @@
       <c r="AN14" s="3"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>412</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -2988,13 +4440,13 @@
       <c r="C15" s="11" t="s">
         <v>524</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>543</v>
+      <c r="D15" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="13" t="s">
         <v>497</v>
       </c>
       <c r="G15" s="3"/>
@@ -3036,16 +4488,16 @@
       <c r="A16" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="13" t="s">
         <v>491</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>67</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E16" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>513</v>
       </c>
       <c r="F16" s="11" t="s">
@@ -3087,22 +4539,22 @@
       <c r="AN16" s="3"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>411</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="13" t="s">
         <v>544</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="13" t="s">
         <v>498</v>
       </c>
       <c r="G17" s="3"/>
@@ -3148,12 +4600,12 @@
         <v>105</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>68</v>
+        <v>560</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="E18" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>514</v>
       </c>
       <c r="F18" s="11" t="s">
@@ -3195,22 +4647,22 @@
       <c r="AN18" s="3"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="13" t="s">
         <v>492</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>143</v>
+        <v>263</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="14" t="s">
         <v>499</v>
       </c>
       <c r="G19" s="3"/>
@@ -3256,12 +4708,12 @@
         <v>108</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="E20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>515</v>
       </c>
       <c r="F20" s="11" t="s">
@@ -3306,19 +4758,19 @@
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>258</v>
+      <c r="C21" s="13" t="s">
+        <v>526</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>545</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>401</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="13" t="s">
         <v>500</v>
       </c>
       <c r="G21" s="3"/>
@@ -3357,19 +4809,19 @@
       <c r="AN21" s="3"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="12" t="s">
         <v>297</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>107</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="E22" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>546</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>400</v>
       </c>
       <c r="F22" s="11" t="s">
@@ -3414,19 +4866,19 @@
       <c r="A23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>303</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>526</v>
+        <v>275</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="12" t="s">
         <v>388</v>
       </c>
       <c r="G23" s="11"/>
@@ -3465,19 +4917,19 @@
       <c r="AN23" s="3"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="E24" s="11" t="s">
+      <c r="C24" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>547</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>337</v>
       </c>
       <c r="F24" s="11" t="s">
@@ -3522,19 +4974,19 @@
       <c r="A25" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>547</v>
+      <c r="C25" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>262</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="13" t="s">
         <v>501</v>
       </c>
       <c r="G25" s="3"/>
@@ -3573,22 +5025,22 @@
       <c r="AN25" s="3"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="12" t="s">
         <v>480</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>435</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>353</v>
+        <v>293</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>281</v>
-      </c>
-      <c r="E26" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>516</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="9" t="s">
         <v>502</v>
       </c>
       <c r="G26" s="3"/>
@@ -3630,19 +5082,19 @@
       <c r="A27" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>351</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="C27" s="12" t="s">
+        <v>527</v>
+      </c>
+      <c r="D27" s="16" t="s">
         <v>548</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="12" t="s">
         <v>367</v>
       </c>
       <c r="G27" s="3"/>
@@ -3681,19 +5133,19 @@
       <c r="AN27" s="3"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="13" t="s">
         <v>481</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>414</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="E28" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>464</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>311</v>
       </c>
       <c r="F28" s="11" t="s">
@@ -3738,19 +5190,19 @@
       <c r="A29" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>317</v>
+      <c r="C29" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>549</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="12" t="s">
         <v>370</v>
       </c>
       <c r="G29" s="3"/>
@@ -3789,19 +5241,19 @@
       <c r="AN29" s="3"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="13" t="s">
         <v>482</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>422</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="E30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>312</v>
       </c>
       <c r="F30" s="11" t="s">
@@ -3843,22 +5295,22 @@
       <c r="AN30" s="3"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>316</v>
+      <c r="C31" s="12" t="s">
+        <v>324</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>440</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="12" t="s">
         <v>372</v>
       </c>
       <c r="G31" s="3"/>
@@ -3897,19 +5349,19 @@
       <c r="AN31" s="3"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="12" t="s">
         <v>413</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="C32" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>550</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="12" t="s">
         <v>313</v>
       </c>
       <c r="F32" s="11" t="s">
@@ -3951,22 +5403,22 @@
       <c r="AN32" s="3"/>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>324</v>
+      <c r="C33" s="12" t="s">
+        <v>345</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>339</v>
+        <v>470</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="12" t="s">
         <v>503</v>
       </c>
       <c r="G33" s="3"/>
@@ -4005,22 +5457,22 @@
       <c r="AN33" s="3"/>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="13" t="s">
         <v>485</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="E34" s="11" t="s">
+      <c r="C34" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>551</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G34" s="3"/>
@@ -4062,19 +5514,19 @@
       <c r="A35" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="12" t="s">
         <v>327</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>551</v>
+        <v>99</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>460</v>
       </c>
       <c r="E35" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="12" t="s">
         <v>387</v>
       </c>
       <c r="G35" s="3"/>
@@ -4113,19 +5565,19 @@
       <c r="AN35" s="3"/>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="12" t="s">
         <v>450</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>470</v>
-      </c>
-      <c r="E36" s="11" t="s">
+      <c r="C36" s="13" t="s">
+        <v>529</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>552</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>333</v>
       </c>
       <c r="F36" s="11" t="s">
@@ -4170,17 +5622,17 @@
       <c r="A37" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>552</v>
+      <c r="C37" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="E37" s="11"/>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="12" t="s">
         <v>386</v>
       </c>
       <c r="G37" s="3"/>
@@ -4219,17 +5671,17 @@
       <c r="AN37" s="3"/>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="12" t="s">
         <v>451</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>529</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>460</v>
+      <c r="C38" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>300</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11" t="s">
@@ -4271,20 +5723,20 @@
       <c r="AN38" s="3"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="12" t="s">
         <v>329</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>553</v>
+        <v>292</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>408</v>
       </c>
       <c r="E39" s="11"/>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="12" t="s">
         <v>504</v>
       </c>
       <c r="G39" s="3"/>
@@ -4323,17 +5775,17 @@
       <c r="AN39" s="3"/>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="12" t="s">
         <v>452</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>426</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>79</v>
+        <v>530</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>553</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11" t="s">
@@ -4376,17 +5828,17 @@
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>292</v>
+      <c r="C41" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>300</v>
+        <v>448</v>
       </c>
       <c r="E41" s="11"/>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="12" t="s">
         <v>384</v>
       </c>
       <c r="G41" s="3"/>
@@ -4430,10 +5882,10 @@
         <v>330</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>530</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>408</v>
+        <v>392</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>554</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="11" t="s">
@@ -4477,14 +5929,14 @@
     <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="11"/>
-      <c r="C43" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>554</v>
+      <c r="C43" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>405</v>
       </c>
       <c r="E43" s="3"/>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="12" t="s">
         <v>383</v>
       </c>
       <c r="G43" s="3"/>
@@ -4525,11 +5977,11 @@
     <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="11"/>
-      <c r="C44" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>448</v>
+      <c r="C44" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="11" t="s">
@@ -4573,14 +6025,14 @@
     <row r="45" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>555</v>
+      <c r="C45" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>421</v>
       </c>
       <c r="E45" s="3"/>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="12" t="s">
         <v>382</v>
       </c>
       <c r="G45" s="3"/>
@@ -4621,11 +6073,11 @@
     <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>405</v>
+      <c r="C46" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>325</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="11" t="s">
@@ -4669,11 +6121,11 @@
     <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>
       <c r="B47" s="3"/>
-      <c r="C47" s="3" t="s">
-        <v>532</v>
+      <c r="C47" s="9" t="s">
+        <v>533</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>318</v>
+        <v>415</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="11" t="s">
@@ -4717,14 +6169,14 @@
     <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A48" s="11"/>
       <c r="B48" s="3"/>
-      <c r="C48" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>421</v>
+      <c r="C48" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="E48" s="3"/>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="12" t="s">
         <v>381</v>
       </c>
       <c r="G48" s="3"/>
@@ -4766,10 +6218,10 @@
       <c r="A49" s="11"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>325</v>
+        <v>404</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="11" t="s">
@@ -4813,14 +6265,14 @@
     <row r="50" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A50" s="11"/>
       <c r="B50" s="3"/>
-      <c r="C50" s="11" t="s">
-        <v>363</v>
+      <c r="C50" s="12" t="s">
+        <v>347</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>415</v>
+        <v>458</v>
       </c>
       <c r="E50" s="3"/>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="12" t="s">
         <v>389</v>
       </c>
       <c r="G50" s="3"/>
@@ -4862,10 +6314,10 @@
       <c r="A51" s="11"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>319</v>
+        <v>535</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>323</v>
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="11" t="s">
@@ -4909,14 +6361,14 @@
     <row r="52" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A52" s="11"/>
       <c r="B52" s="3"/>
-      <c r="C52" s="11" t="s">
-        <v>347</v>
+      <c r="C52" s="12" t="s">
+        <v>350</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>404</v>
+        <v>459</v>
       </c>
       <c r="E52" s="3"/>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="12" t="s">
         <v>391</v>
       </c>
       <c r="G52" s="3"/>
@@ -4958,10 +6410,10 @@
       <c r="A53" s="11"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>458</v>
+        <v>536</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>555</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="11" t="s">
@@ -5006,10 +6458,10 @@
       <c r="A54" s="11"/>
       <c r="B54" s="3"/>
       <c r="C54" s="11" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>323</v>
+        <v>406</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="11" t="s">
@@ -5053,14 +6505,14 @@
     <row r="55" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A55" s="11"/>
       <c r="B55" s="3"/>
-      <c r="C55" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>459</v>
+      <c r="C55" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>308</v>
       </c>
       <c r="E55" s="3"/>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="12" t="s">
         <v>445</v>
       </c>
       <c r="G55" s="11"/>
@@ -5102,10 +6554,10 @@
       <c r="A56" s="11"/>
       <c r="B56" s="3"/>
       <c r="C56" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>556</v>
+        <v>537</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>407</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="11" t="s">
@@ -5149,14 +6601,14 @@
     <row r="57" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A57" s="11"/>
       <c r="B57" s="3"/>
-      <c r="C57" s="11" t="s">
-        <v>355</v>
+      <c r="C57" s="12" t="s">
+        <v>362</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>406</v>
+        <v>438</v>
       </c>
       <c r="E57" s="11"/>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="12" t="s">
         <v>509</v>
       </c>
       <c r="G57" s="11"/>
@@ -5198,10 +6650,10 @@
       <c r="A58" s="11"/>
       <c r="B58" s="3"/>
       <c r="C58" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>308</v>
+        <v>433</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>322</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="11"/>
@@ -5243,11 +6695,11 @@
     <row r="59" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A59" s="11"/>
       <c r="B59" s="3"/>
-      <c r="C59" s="11" t="s">
-        <v>362</v>
+      <c r="C59" s="12" t="s">
+        <v>361</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>407</v>
+        <v>437</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="11"/>
@@ -5290,10 +6742,10 @@
       <c r="A60" s="11"/>
       <c r="B60" s="3"/>
       <c r="C60" s="11" t="s">
-        <v>433</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>438</v>
+        <v>456</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>342</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="11"/>
@@ -5335,11 +6787,11 @@
     <row r="61" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A61" s="11"/>
       <c r="B61" s="3"/>
-      <c r="C61" s="11" t="s">
-        <v>361</v>
+      <c r="C61" s="12" t="s">
+        <v>455</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>322</v>
+        <v>436</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="11"/>
@@ -5381,11 +6833,11 @@
     <row r="62" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A62" s="11"/>
       <c r="B62" s="3"/>
-      <c r="C62" s="11" t="s">
-        <v>456</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>437</v>
+      <c r="C62" s="19" t="s">
+        <v>419</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>341</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="11"/>
@@ -5427,11 +6879,11 @@
     <row r="63" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A63" s="11"/>
       <c r="B63" s="3"/>
-      <c r="C63" s="11" t="s">
-        <v>455</v>
+      <c r="C63" s="19" t="s">
+        <v>314</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>342</v>
+        <v>395</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="11"/>
@@ -5473,11 +6925,11 @@
     <row r="64" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A64" s="11"/>
       <c r="B64" s="3"/>
-      <c r="C64" s="11" t="s">
-        <v>419</v>
+      <c r="C64" s="19" t="s">
+        <v>442</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>436</v>
+        <v>396</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="11"/>
@@ -5519,11 +6971,11 @@
     <row r="65" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A65" s="11"/>
       <c r="B65" s="3"/>
-      <c r="C65" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>341</v>
+      <c r="C65" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>556</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="11"/>
@@ -5565,11 +7017,11 @@
     <row r="66" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A66" s="11"/>
       <c r="B66" s="3"/>
-      <c r="C66" s="11" t="s">
-        <v>442</v>
+      <c r="C66" s="19" t="s">
+        <v>420</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="11"/>
@@ -5611,11 +7063,11 @@
     <row r="67" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A67" s="11"/>
       <c r="B67" s="3"/>
-      <c r="C67" s="11" t="s">
-        <v>320</v>
+      <c r="C67" s="19" t="s">
+        <v>335</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="11"/>
@@ -5657,10 +7109,10 @@
     <row r="68" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A68" s="11"/>
       <c r="B68" s="3"/>
-      <c r="C68" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="D68" s="3" t="s">
+      <c r="C68" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="D68" s="13" t="s">
         <v>557</v>
       </c>
       <c r="E68" s="3"/>
@@ -5703,11 +7155,11 @@
     <row r="69" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A69" s="11"/>
       <c r="B69" s="3"/>
-      <c r="C69" s="11" t="s">
-        <v>335</v>
+      <c r="C69" s="19" t="s">
+        <v>336</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>397</v>
+        <v>82</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
@@ -5749,11 +7201,11 @@
     <row r="70" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A70" s="11"/>
       <c r="B70" s="3"/>
-      <c r="C70" s="11" t="s">
-        <v>443</v>
+      <c r="C70" s="19" t="s">
+        <v>444</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>398</v>
+        <v>81</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -5795,11 +7247,11 @@
     <row r="71" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
-      <c r="C71" s="11" t="s">
-        <v>336</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>558</v>
+      <c r="C71" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>305</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -5841,11 +7293,11 @@
     <row r="72" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
-      <c r="C72" s="11" t="s">
-        <v>444</v>
+      <c r="C72" s="19" t="s">
+        <v>431</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -5887,11 +7339,11 @@
     <row r="73" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
-      <c r="C73" s="11" t="s">
-        <v>332</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>81</v>
+      <c r="C73" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>304</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -5933,11 +7385,9 @@
     <row r="74" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
-      <c r="C74" s="11" t="s">
-        <v>431</v>
-      </c>
+      <c r="C74" s="3"/>
       <c r="D74" s="11" t="s">
-        <v>305</v>
+        <v>394</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -5979,11 +7429,9 @@
     <row r="75" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
-      <c r="C75" s="11" t="s">
-        <v>338</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>84</v>
+      <c r="C75" s="3"/>
+      <c r="D75" s="12" t="s">
+        <v>309</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -6027,7 +7475,7 @@
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="11" t="s">
-        <v>304</v>
+        <v>96</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -6071,7 +7519,7 @@
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="11" t="s">
-        <v>394</v>
+        <v>416</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -6114,8 +7562,8 @@
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="11" t="s">
-        <v>309</v>
+      <c r="D78" s="12" t="s">
+        <v>306</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
@@ -6159,7 +7607,7 @@
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="11" t="s">
-        <v>96</v>
+        <v>417</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -6202,8 +7650,8 @@
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="11" t="s">
-        <v>416</v>
+      <c r="D80" s="12" t="s">
+        <v>307</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -6247,7 +7695,7 @@
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="11" t="s">
-        <v>306</v>
+        <v>429</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -6290,8 +7738,8 @@
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="11" t="s">
-        <v>417</v>
+      <c r="D82" s="12" t="s">
+        <v>334</v>
       </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
@@ -6335,7 +7783,7 @@
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="11" t="s">
-        <v>307</v>
+        <v>432</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
@@ -6378,8 +7826,8 @@
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
-      <c r="D84" s="11" t="s">
-        <v>429</v>
+      <c r="D84" s="12" t="s">
+        <v>360</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
@@ -6423,7 +7871,7 @@
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="11" t="s">
-        <v>334</v>
+        <v>402</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
@@ -6466,8 +7914,8 @@
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
-      <c r="D86" s="11" t="s">
-        <v>432</v>
+      <c r="D86" s="13" t="s">
+        <v>558</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -6511,7 +7959,7 @@
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="11" t="s">
-        <v>360</v>
+        <v>559</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
@@ -6554,8 +8002,8 @@
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
-      <c r="D88" s="11" t="s">
-        <v>402</v>
+      <c r="D88" s="12" t="s">
+        <v>447</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
@@ -6598,9 +8046,7 @@
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
-      <c r="D89" s="3" t="s">
-        <v>559</v>
-      </c>
+      <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -6642,9 +8088,7 @@
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
-      <c r="D90" s="11" t="s">
-        <v>560</v>
-      </c>
+      <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -6686,9 +8130,7 @@
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
-      <c r="D91" s="11" t="s">
-        <v>447</v>
-      </c>
+      <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -10762,7 +12204,6 @@
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
       <c r="E188" s="3"/>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
@@ -10804,7 +12245,6 @@
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
-      <c r="D189" s="3"/>
       <c r="E189" s="3"/>
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
@@ -10844,8 +12284,6 @@
     </row>
     <row r="190" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
       <c r="E190" s="3"/>
       <c r="F190" s="3"/>
       <c r="G190" s="3"/>
@@ -10883,16 +12321,13 @@
       <c r="AM190" s="3"/>
       <c r="AN190" s="3"/>
     </row>
-    <row r="191" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="C191" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H113"/>
   <sheetViews>
@@ -10904,8 +12339,8 @@
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="27.69921875" customWidth="1"/>
-    <col min="3" max="3" width="25.796875" customWidth="1"/>
-    <col min="4" max="4" width="18.296875" customWidth="1"/>
+    <col min="3" max="3" width="25.69921875" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" customWidth="1"/>
     <col min="5" max="5" width="16.69921875" customWidth="1"/>
     <col min="6" max="6" width="35.59765625" customWidth="1"/>
     <col min="7" max="7" width="17.59765625" bestFit="1" customWidth="1"/>
@@ -11987,7 +13422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -12373,7 +13808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -12396,10 +13831,10 @@
       <c r="D1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="12"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -12549,7 +13984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
@@ -12560,15 +13995,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24.796875" customWidth="1"/>
+    <col min="2" max="2" width="24.69921875" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="16.59765625" customWidth="1"/>
-    <col min="5" max="6" width="16.296875" customWidth="1"/>
-    <col min="7" max="7" width="14.796875" customWidth="1"/>
+    <col min="5" max="6" width="16.19921875" customWidth="1"/>
+    <col min="7" max="7" width="14.69921875" customWidth="1"/>
     <col min="8" max="8" width="22.59765625" customWidth="1"/>
     <col min="9" max="9" width="23.09765625" customWidth="1"/>
     <col min="10" max="10" width="27.09765625" customWidth="1"/>
-    <col min="11" max="11" width="18.796875" customWidth="1"/>
+    <col min="11" max="11" width="18.69921875" customWidth="1"/>
     <col min="12" max="12" width="38" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>